<commit_message>
Mise à jour des documents
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_S1-Eq1.xlsx
+++ b/Documents/Feuille_de_temps_S1-Eq1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AWT\NovaGo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC09BCD-581A-4830-B046-EDA315EE965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE9EE13A-8C22-4D60-ABA2-CC7AA0A08D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
   <si>
     <t>Temps</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Félix</t>
+  </si>
+  <si>
+    <t>environ 12h</t>
   </si>
 </sst>
 </file>
@@ -237,7 +240,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -539,10 +542,10 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -593,8 +596,8 @@
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9">
-        <v>0</v>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
@@ -713,7 +716,7 @@
       <selection activeCell="C2" sqref="C2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
   </cols>
@@ -782,7 +785,7 @@
       <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
   </cols>
@@ -855,7 +858,7 @@
       <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -7905,7 +7908,7 @@
       <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>

</xml_diff>